<commit_message>
updated PerfCompare.xlsx with agressive speed flow settings
</commit_message>
<xml_diff>
--- a/doc/PerfCompare.xlsx
+++ b/doc/PerfCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Revision</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Flow settings</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -145,6 +142,66 @@
   </si>
   <si>
     <t>Default, target Fmax=150 MHz</t>
+  </si>
+  <si>
+    <t>Aggressive performance, target Fmax=250 MHz</t>
+  </si>
+  <si>
+    <t>229.89 MHz</t>
+  </si>
+  <si>
+    <t>2,503</t>
+  </si>
+  <si>
+    <t>2,102</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>2,810</t>
+  </si>
+  <si>
+    <t>2,137</t>
+  </si>
+  <si>
+    <t>2137</t>
+  </si>
+  <si>
+    <t>226.04 MHz</t>
+  </si>
+  <si>
+    <t>221.68 MHz</t>
+  </si>
+  <si>
+    <t>1,970</t>
+  </si>
+  <si>
+    <t>1,689</t>
+  </si>
+  <si>
+    <t>1,811</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>2,373</t>
+  </si>
+  <si>
+    <t>2,002</t>
+  </si>
+  <si>
+    <t>2,017</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>213.08 MHz</t>
+  </si>
+  <si>
+    <t>Area, target Fmax=250 MHz</t>
   </si>
 </sst>
 </file>
@@ -177,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -381,7 +438,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -397,34 +454,21 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -433,17 +477,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -454,22 +487,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -477,50 +501,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -532,7 +538,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,14 +556,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -558,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -862,359 +875,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="16.7109375" customWidth="1"/>
+    <col min="2" max="13" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="43"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="49"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="46"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="40"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="18"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="24"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="55"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="24"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="26" t="s">
+      <c r="C20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="D20" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="30"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="30"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
+      <c r="F20" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
+  <mergeCells count="9">
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>

</xml_diff>

<commit_message>
added data for area optimization flow settings
</commit_message>
<xml_diff>
--- a/doc/PerfCompare.xlsx
+++ b/doc/PerfCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Revision</t>
   </si>
@@ -201,7 +201,13 @@
     <t>213.08 MHz</t>
   </si>
   <si>
-    <t>Area, target Fmax=250 MHz</t>
+    <t>Area, target Fmax=150 MHz</t>
+  </si>
+  <si>
+    <t>168.95 MHz</t>
+  </si>
+  <si>
+    <t>162.02 MHz</t>
   </si>
 </sst>
 </file>
@@ -538,6 +544,24 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,24 +578,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -878,7 +884,7 @@
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,20 +937,20 @@
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="43"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -967,64 +973,64 @@
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="47" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="47" t="s">
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="49"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="40"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="44" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="44" t="s">
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="40"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="46"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1054,8 +1060,12 @@
       <c r="I9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="J9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
@@ -1087,8 +1097,12 @@
       <c r="I10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
+      <c r="J10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
@@ -1120,8 +1134,12 @@
       <c r="I11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
@@ -1153,8 +1171,12 @@
       <c r="I12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
+      <c r="J12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
@@ -1186,27 +1208,31 @@
       <c r="I13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
+      <c r="J13" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="L13" s="22"/>
       <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="40"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="46"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1321,8 +1347,12 @@
       <c r="I20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30"/>
+      <c r="J20" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="L20" s="31"/>
       <c r="M20" s="32"/>
     </row>

</xml_diff>

<commit_message>
added new perf data
</commit_message>
<xml_diff>
--- a/doc/PerfCompare.xlsx
+++ b/doc/PerfCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>Revision</t>
   </si>
@@ -208,6 +208,27 @@
   </si>
   <si>
     <t>162.02 MHz</t>
+  </si>
+  <si>
+    <t>216.31 MHz</t>
+  </si>
+  <si>
+    <t>1,934</t>
+  </si>
+  <si>
+    <t>1,655</t>
+  </si>
+  <si>
+    <t>1,776</t>
+  </si>
+  <si>
+    <t>1776</t>
+  </si>
+  <si>
+    <t>211.6 MHz</t>
+  </si>
+  <si>
+    <t>ea266541b1ecebd0a18282bac76adb4200bea96b</t>
   </si>
 </sst>
 </file>
@@ -240,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -489,11 +510,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,6 +641,38 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,31 +682,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -884,13 +998,14 @@
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="16.7109375" customWidth="1"/>
+    <col min="2" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -917,40 +1032,46 @@
       <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>18</v>
+      <c r="L3" s="42" t="s">
+        <v>16</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="46"/>
+      <c r="L4" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="46"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -963,9 +1084,9 @@
       <c r="F5" s="8"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="38"/>
       <c r="L5" s="8"/>
       <c r="M5" s="7"/>
     </row>
@@ -973,64 +1094,66 @@
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="38" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="38" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="56"/>
+      <c r="L6" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="40"/>
+      <c r="M6" s="54"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="41" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="41" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="43"/>
+      <c r="M7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="48"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1045,7 +1168,7 @@
       <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -1060,14 +1183,18 @@
       <c r="I9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="M9" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -1097,14 +1224,18 @@
       <c r="I10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="M10" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
@@ -1134,14 +1265,18 @@
       <c r="I11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="M11" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
@@ -1171,14 +1306,18 @@
       <c r="I12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="M12" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
@@ -1208,31 +1347,35 @@
       <c r="I13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="24"/>
+      <c r="L13" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="23" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1246,10 +1389,10 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="27"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
@@ -1263,9 +1406,9 @@
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1280,9 +1423,9 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1297,12 +1440,12 @@
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1314,9 +1457,9 @@
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1335,7 +1478,7 @@
       <c r="E20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="30" t="s">
@@ -1347,14 +1490,18 @@
       <c r="I20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="M20" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
@@ -1368,24 +1515,30 @@
       <c r="G21" s="35"/>
       <c r="H21" s="36"/>
       <c r="I21" s="37"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="37"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="B8:M8"/>
+  <mergeCells count="14">
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="C8:M8"/>
     <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B4:M4"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated PerfCompare.xlsx, changed compilation settings for systolic design
</commit_message>
<xml_diff>
--- a/doc/PerfCompare.xlsx
+++ b/doc/PerfCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
   <si>
     <t>Revision</t>
   </si>
@@ -229,6 +229,60 @@
   </si>
   <si>
     <t>ea266541b1ecebd0a18282bac76adb4200bea96b</t>
+  </si>
+  <si>
+    <t>0409e659a77db7a08db3c0e6cb88c785c5f40d0b</t>
+  </si>
+  <si>
+    <t>Systolic, Non-symmetric</t>
+  </si>
+  <si>
+    <t>Systolic, Symmetric</t>
+  </si>
+  <si>
+    <t>2,023</t>
+  </si>
+  <si>
+    <t>2,019</t>
+  </si>
+  <si>
+    <t>1,661</t>
+  </si>
+  <si>
+    <t>1661</t>
+  </si>
+  <si>
+    <t>185.25 MHz</t>
+  </si>
+  <si>
+    <t>3,163</t>
+  </si>
+  <si>
+    <t>3,065</t>
+  </si>
+  <si>
+    <t>2,702</t>
+  </si>
+  <si>
+    <t>2702</t>
+  </si>
+  <si>
+    <t>171.32 MHz</t>
+  </si>
+  <si>
+    <t>3,053</t>
+  </si>
+  <si>
+    <t>194.59 MHz</t>
+  </si>
+  <si>
+    <t>2,010</t>
+  </si>
+  <si>
+    <t>2,006</t>
+  </si>
+  <si>
+    <t>193.54 MHz</t>
   </si>
 </sst>
 </file>
@@ -261,7 +315,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -586,11 +640,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -642,7 +851,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -692,6 +900,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,16 +1278,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M21"/>
+  <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="16.7109375" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1041,7 +1325,7 @@
       <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="41" t="s">
         <v>16</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -1052,26 +1336,26 @@
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="44" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="44" t="s">
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="45" t="s">
+      <c r="K4" s="45"/>
+      <c r="L4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="46"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1085,7 +1369,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="43"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="38"/>
       <c r="L5" s="8"/>
       <c r="M5" s="7"/>
@@ -1094,66 +1378,66 @@
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="52" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="55" t="s">
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="53" t="s">
+      <c r="K6" s="55"/>
+      <c r="L6" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="54"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="49" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="50" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="51"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="48"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1192,7 +1476,7 @@
       <c r="L9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="40" t="s">
+      <c r="M9" s="39" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1233,7 +1517,7 @@
       <c r="L10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="40" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1274,7 +1558,7 @@
       <c r="L11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="40" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1315,7 +1599,7 @@
       <c r="L12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="40" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1362,20 +1646,20 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="48"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1445,7 +1729,7 @@
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1737,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="18"/>
@@ -1478,7 +1762,7 @@
       <c r="E20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="30" t="s">
@@ -1520,11 +1804,409 @@
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
     </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="59"/>
+      <c r="B23" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="82"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="100"/>
+      <c r="D24" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="100"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="73"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="87"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="74"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="66"/>
+      <c r="M26" s="75"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="50"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="75"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="76"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="91" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="91">
+        <v>3.1509999999999998</v>
+      </c>
+      <c r="F29" s="95"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="77"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="88"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="77"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="88"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="77"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="88"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="77"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="94" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="95"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="77"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="76"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="90"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="78"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="92"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="78"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="92"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="88"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="78"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="92"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="92"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="78"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="92"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="78"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="88"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="68"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="77"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="98"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="96"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="80"/>
+      <c r="I41" s="80"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="80"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="22">
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="C8:M8"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B6:E6"/>
@@ -1538,7 +2220,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>